<commit_message>
format the paper and complete the part of abstract
</commit_message>
<xml_diff>
--- a/Mypaper/tables/4.6风险因素影响统计分析.xlsx
+++ b/Mypaper/tables/4.6风险因素影响统计分析.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12450"/>
+    <workbookView windowWidth="24225" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>需求不明确风险因素R</t>
     </r>
     <r>
@@ -69,6 +76,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>需求蔓延风险因素R</t>
     </r>
     <r>
@@ -95,6 +109,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>需求持续变更风险因素R</t>
     </r>
     <r>
@@ -121,6 +142,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>技术过于新颖风险因素R</t>
     </r>
     <r>
@@ -147,6 +175,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>网络攻击风险因素R</t>
     </r>
     <r>
@@ -173,6 +208,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>开发工具的选择风险因素R</t>
     </r>
     <r>
@@ -199,6 +241,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>开发语言的选择风险因素R</t>
     </r>
     <r>
@@ -223,6 +271,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>人员离职风险因素R</t>
     </r>
     <r>
@@ -249,6 +304,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>开发人员的团队协作能力风险因素R</t>
     </r>
     <r>
@@ -275,6 +337,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>项目成员缺少主动性风险因素R</t>
     </r>
     <r>
@@ -301,6 +370,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>项目经理的过于强势风险因素R</t>
     </r>
     <r>
@@ -327,6 +403,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>团队成员沟通风险因素R</t>
     </r>
     <r>
@@ -353,6 +436,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>项目经理专业性不强风险因素R</t>
     </r>
     <r>
@@ -379,6 +469,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>缺乏公司高层支持风险因素R</t>
     </r>
     <r>
@@ -405,6 +502,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>用户预期过高风险因素R</t>
     </r>
     <r>
@@ -431,6 +535,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>用户与软件开发人员有冲突风险因素R</t>
     </r>
     <r>
@@ -457,6 +568,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>用户参与度不足风险因素R</t>
     </r>
     <r>
@@ -483,6 +601,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>供应商延迟交付风险因素R</t>
     </r>
     <r>
@@ -509,6 +634,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>供应商技术支持力度不够风险因素R</t>
     </r>
     <r>
@@ -535,6 +667,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>目资源向其他项目偏移风险因素R</t>
     </r>
     <r>
@@ -561,6 +700,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>缺少软件经验教训文档风险因素R</t>
     </r>
     <r>
@@ -587,6 +733,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>中国Android取消授权风险因素R</t>
     </r>
     <r>
@@ -613,6 +766,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>应用无法上架应用市场风险因素R</t>
     </r>
     <r>
@@ -644,18 +804,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,6 +831,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -685,53 +845,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -752,11 +866,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -768,32 +913,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -815,7 +939,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -853,61 +1006,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -917,146 +1190,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1075,24 +1215,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1121,36 +1254,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1175,6 +1278,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1190,177 +1317,162 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1714,7 +1826,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A1" sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1731,16 +1843,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1748,16 +1860,16 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="G2" t="s">
@@ -1768,19 +1880,19 @@
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:8">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="1">
         <v>201</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="1">
         <v>39</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3">
@@ -1797,19 +1909,19 @@
       </c>
     </row>
     <row r="4" ht="15" spans="1:8">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="1">
         <v>223</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="1">
         <v>18</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4">
@@ -1826,19 +1938,19 @@
       </c>
     </row>
     <row r="5" ht="15" spans="1:8">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="1">
         <v>215</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="1">
         <v>26</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5">
@@ -1855,19 +1967,19 @@
       </c>
     </row>
     <row r="6" ht="15" spans="1:8">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="1">
         <v>69</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="1">
         <v>105</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="1">
         <v>66</v>
       </c>
       <c r="F6">
@@ -1884,19 +1996,19 @@
       </c>
     </row>
     <row r="7" ht="15" spans="1:8">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="1">
         <v>11</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="1">
         <v>87</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="1">
         <v>97</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="1">
         <v>47</v>
       </c>
       <c r="F7">
@@ -1913,19 +2025,19 @@
       </c>
     </row>
     <row r="8" ht="15" spans="1:8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="1">
         <v>13</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="1">
         <v>117</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="1">
         <v>109</v>
       </c>
       <c r="F8">
@@ -1942,19 +2054,19 @@
       </c>
     </row>
     <row r="9" ht="15" spans="1:8">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="1">
         <v>11</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="1">
         <v>116</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="1">
         <v>113</v>
       </c>
       <c r="F9">
@@ -1971,19 +2083,19 @@
       </c>
     </row>
     <row r="10" ht="15" spans="1:8">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="1">
         <v>189</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="1">
         <v>37</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="1">
         <v>16</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="1">
         <v>0</v>
       </c>
       <c r="F10">
@@ -2000,19 +2112,19 @@
       </c>
     </row>
     <row r="11" ht="15" spans="1:8">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="1">
         <v>96</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="1">
         <v>106</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="1">
         <v>37</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="1">
         <v>3</v>
       </c>
       <c r="F11">
@@ -2029,19 +2141,19 @@
       </c>
     </row>
     <row r="12" ht="15" spans="1:8">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="1">
         <v>72</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="1">
         <v>92</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="1">
         <v>76</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="1">
         <v>2</v>
       </c>
       <c r="F12">
@@ -2058,19 +2170,19 @@
       </c>
     </row>
     <row r="13" ht="15" spans="1:8">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="1">
         <v>32</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="1">
         <v>96</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="1">
         <v>89</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="1">
         <v>25</v>
       </c>
       <c r="F13">
@@ -2087,19 +2199,19 @@
       </c>
     </row>
     <row r="14" ht="15" spans="1:8">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="1">
         <v>236</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="1">
         <v>5</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="F14">
@@ -2116,19 +2228,19 @@
       </c>
     </row>
     <row r="15" ht="15" spans="1:8">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="1">
         <v>18</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="1">
         <v>87</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="1">
         <v>75</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="1">
         <v>62</v>
       </c>
       <c r="F15">
@@ -2145,48 +2257,48 @@
       </c>
     </row>
     <row r="16" ht="15" spans="1:8">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="1">
         <v>183</v>
       </c>
-      <c r="C16" s="5">
-        <v>54</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="C16" s="1">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1">
         <v>2</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="1">
         <v>0</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>898</v>
+        <v>907</v>
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
-        <v>3.71074380165289</v>
+        <v>3.74793388429752</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:8">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="1">
         <v>21</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="1">
         <v>97</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="1">
         <v>76</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="1">
         <v>48</v>
       </c>
       <c r="F17">
@@ -2203,19 +2315,19 @@
       </c>
     </row>
     <row r="18" ht="15" spans="1:8">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="1">
         <v>9</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="1">
         <v>25</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="1">
         <v>97</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="1">
         <v>111</v>
       </c>
       <c r="F18">
@@ -2232,19 +2344,19 @@
       </c>
     </row>
     <row r="19" ht="15" spans="1:8">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="1">
         <v>7</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="1">
         <v>23</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="1">
         <v>117</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="1">
         <v>95</v>
       </c>
       <c r="F19">
@@ -2261,19 +2373,19 @@
       </c>
     </row>
     <row r="20" ht="15" spans="1:8">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="1">
         <v>135</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="1">
         <v>88</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="1">
         <v>17</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="1">
         <v>2</v>
       </c>
       <c r="F20">
@@ -2290,19 +2402,19 @@
       </c>
     </row>
     <row r="21" ht="15" spans="1:8">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="1">
         <v>158</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="1">
         <v>64</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="1">
         <v>16</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="1">
         <v>4</v>
       </c>
       <c r="F21">
@@ -2319,19 +2431,19 @@
       </c>
     </row>
     <row r="22" ht="15" spans="1:8">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="1">
         <v>192</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="1">
         <v>42</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="1">
         <v>5</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="1">
         <v>3</v>
       </c>
       <c r="F22">
@@ -2348,19 +2460,19 @@
       </c>
     </row>
     <row r="23" ht="15" spans="1:8">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="1">
         <v>10</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="1">
         <v>36</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="1">
         <v>156</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="1">
         <v>40</v>
       </c>
       <c r="F23">
@@ -2377,19 +2489,19 @@
       </c>
     </row>
     <row r="24" ht="15" spans="1:8">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="1">
         <v>239</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="1">
         <v>3</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="1">
         <v>0</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="1">
         <v>0</v>
       </c>
       <c r="F24">
@@ -2406,19 +2518,19 @@
       </c>
     </row>
     <row r="25" ht="15" spans="1:8">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="1">
         <v>10</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="1">
         <v>78</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="1">
         <v>89</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="1">
         <v>65</v>
       </c>
       <c r="F25">

</xml_diff>